<commit_message>
Muharrem - TestCase Add
</commit_message>
<xml_diff>
--- a/src/test/java/Resources/mMarktTestCases.xlsx
+++ b/src/test/java/Resources/mMarktTestCases.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkara\IdeaProjects\MediaMarktWebsiteTesting\src\test\java\Resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sayfa1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,21 +24,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="69">
-  <si>
-    <t xml:space="preserve">TestID</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="97">
+  <si>
+    <t>TestID</t>
   </si>
   <si>
     <t xml:space="preserve">Test case category </t>
   </si>
   <si>
-    <t xml:space="preserve">Description /Summary</t>
+    <t>Description /Summary</t>
   </si>
   <si>
     <t xml:space="preserve">Environment </t>
   </si>
   <si>
-    <t xml:space="preserve">Steps</t>
+    <t>Steps</t>
   </si>
   <si>
     <t xml:space="preserve">Test data </t>
@@ -43,152 +47,152 @@
     <t xml:space="preserve">Expected result </t>
   </si>
   <si>
-    <t xml:space="preserve">Actual Result</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Result</t>
-  </si>
-  <si>
-    <t xml:space="preserve">İbrahimFigen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Positive test case</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The user can select the desired headset and come to the payment page.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.mediamarkt.com.tr/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Navigate to MediaMarkt</t>
+    <t>Actual Result</t>
+  </si>
+  <si>
+    <t>Test Result</t>
+  </si>
+  <si>
+    <t>İbrahimFigen</t>
+  </si>
+  <si>
+    <t>Positive test case</t>
+  </si>
+  <si>
+    <t>The user can select the desired headset and come to the payment page.</t>
+  </si>
+  <si>
+    <t>https://www.mediamarkt.com.tr/</t>
+  </si>
+  <si>
+    <t>1. Navigate to MediaMarkt</t>
   </si>
   <si>
     <t xml:space="preserve">The MediaMarkt page should open
 </t>
   </si>
   <si>
-    <t xml:space="preserve">successful</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PASSED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.Verify that you are on the home page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The user must be verified to be on the homepage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.Type the product in the search box and click enter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The user should be able to search with the search box</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.Click on the random product</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The user should be able to choose a random product.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.Click add to cart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The user should be able to click add to cart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.Click on the additional insurance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User should be able to click on additional insurance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.Add to cart and click continue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User should be able to click add to cart and continue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.Click on the go to cart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User should be able to click go to cart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.Click on the continue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User should be able to click continue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.Click on the continue without registration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User should be able to click continue without registration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11.Fill in the address form and save</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User should be able to fill and save the Address form</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12.Click on the continue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cucumber type test case</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gherkin language</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given Navigate to MediaMarkt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">When Verify that you are on the home page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">And Type the product in the search box and click enter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">And Click on the random product</t>
-  </si>
-  <si>
-    <t xml:space="preserve">And Click add to cart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">And Click on the additional insurance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">And Add to cart and click continue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">And Click on the go to cart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">And Click on the continue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">And Click on the continue without registration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">And Fill in the address form and save</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OmerAvci</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kendi testinizin açıklaması</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hakan Tasdelen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Positive Test Case</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The user should be able to download the latest issue of the magazine from the website with a single click.</t>
+    <t>successful</t>
+  </si>
+  <si>
+    <t>PASSED</t>
+  </si>
+  <si>
+    <t>2.Verify that you are on the home page</t>
+  </si>
+  <si>
+    <t>The user must be verified to be on the homepage</t>
+  </si>
+  <si>
+    <t>3.Type the product in the search box and click enter</t>
+  </si>
+  <si>
+    <t>The user should be able to search with the search box</t>
+  </si>
+  <si>
+    <t>4.Click on the random product</t>
+  </si>
+  <si>
+    <t>The user should be able to choose a random product.</t>
+  </si>
+  <si>
+    <t>5.Click add to cart</t>
+  </si>
+  <si>
+    <t>The user should be able to click add to cart</t>
+  </si>
+  <si>
+    <t>6.Click on the additional insurance</t>
+  </si>
+  <si>
+    <t>User should be able to click on additional insurance</t>
+  </si>
+  <si>
+    <t>7.Add to cart and click continue</t>
+  </si>
+  <si>
+    <t>User should be able to click add to cart and continue</t>
+  </si>
+  <si>
+    <t>8.Click on the go to cart</t>
+  </si>
+  <si>
+    <t>User should be able to click go to cart</t>
+  </si>
+  <si>
+    <t>9.Click on the continue</t>
+  </si>
+  <si>
+    <t>User should be able to click continue</t>
+  </si>
+  <si>
+    <t>10.Click on the continue without registration</t>
+  </si>
+  <si>
+    <t>User should be able to click continue without registration</t>
+  </si>
+  <si>
+    <t>11.Fill in the address form and save</t>
+  </si>
+  <si>
+    <t>User should be able to fill and save the Address form</t>
+  </si>
+  <si>
+    <t>12.Click on the continue</t>
+  </si>
+  <si>
+    <t>Cucumber type test case</t>
+  </si>
+  <si>
+    <t>Gherkin language</t>
+  </si>
+  <si>
+    <t>Given Navigate to MediaMarkt</t>
+  </si>
+  <si>
+    <t>When Verify that you are on the home page</t>
+  </si>
+  <si>
+    <t>And Type the product in the search box and click enter</t>
+  </si>
+  <si>
+    <t>And Click on the random product</t>
+  </si>
+  <si>
+    <t>And Click add to cart</t>
+  </si>
+  <si>
+    <t>And Click on the additional insurance</t>
+  </si>
+  <si>
+    <t>And Add to cart and click continue</t>
+  </si>
+  <si>
+    <t>And Click on the go to cart</t>
+  </si>
+  <si>
+    <t>And Click on the continue</t>
+  </si>
+  <si>
+    <t>And Click on the continue without registration</t>
+  </si>
+  <si>
+    <t>And Fill in the address form and save</t>
+  </si>
+  <si>
+    <t>OmerAvci</t>
+  </si>
+  <si>
+    <t>Kendi testinizin açıklaması</t>
+  </si>
+  <si>
+    <t>Hakan Tasdelen</t>
+  </si>
+  <si>
+    <t>Positive Test Case</t>
+  </si>
+  <si>
+    <t>The user should be able to download the latest issue of the magazine from the website with a single click.</t>
   </si>
   <si>
     <t xml:space="preserve">The MediaMarkt page should be open
@@ -199,47 +203,128 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">The user should be able to go to bottom of page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4. Click on the icon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The user should be click on the Media Trend icon</t>
+    <t>The user should be able to go to bottom of page</t>
+  </si>
+  <si>
+    <t>4. Click on the icon</t>
+  </si>
+  <si>
+    <t>The user should be click on the Media Trend icon</t>
   </si>
   <si>
     <t xml:space="preserve">5. Assert to opened window </t>
   </si>
   <si>
-    <t xml:space="preserve">The user should be able to verify that the window contains a download link</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6. Download the magazine to your local</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The user can be download the magazine to own local</t>
-  </si>
-  <si>
-    <t xml:space="preserve">And Click the media trend</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Then Click the download media trend magazine and assert it</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OrcunIlgen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kendi nameniz</t>
+    <t>The user should be able to verify that the window contains a download link</t>
+  </si>
+  <si>
+    <t>6. Download the magazine to your local</t>
+  </si>
+  <si>
+    <t>The user can be download the magazine to own local</t>
+  </si>
+  <si>
+    <t>And Click the media trend</t>
+  </si>
+  <si>
+    <t>Then Click the download media trend magazine and assert it</t>
+  </si>
+  <si>
+    <t>OrcunIlgen</t>
+  </si>
+  <si>
+    <t>kendi nameniz</t>
+  </si>
+  <si>
+    <t>Muharrem Karapazar</t>
+  </si>
+  <si>
+    <t>User can make stock inquiry with product number</t>
+  </si>
+  <si>
+    <t>2. Verify that you are on the home page</t>
+  </si>
+  <si>
+    <t>3. Click on Personal Care products</t>
+  </si>
+  <si>
+    <t>4. Click on Male Grooming products</t>
+  </si>
+  <si>
+    <t>5. Sort products from most expensive to least expensive</t>
+  </si>
+  <si>
+    <t>6. Choose the most expensive product</t>
+  </si>
+  <si>
+    <t>7. Get Item No (serial number)</t>
+  </si>
+  <si>
+    <t>8. Click on Stock Inquiry Button</t>
+  </si>
+  <si>
+    <t>9. Make a stock inquiry of the product</t>
+  </si>
+  <si>
+    <t>10. Stock information</t>
+  </si>
+  <si>
+    <t>Given Click on Personal Care products</t>
+  </si>
+  <si>
+    <t>And Click on Male Grooming products</t>
+  </si>
+  <si>
+    <t>And Sort products from most expensive to least expensive</t>
+  </si>
+  <si>
+    <t>And Choose the most expensive product</t>
+  </si>
+  <si>
+    <t>And Get Item No (serial number)</t>
+  </si>
+  <si>
+    <t>And Click on Stock Inquiry Button</t>
+  </si>
+  <si>
+    <t>And Make a stock inquiry of the product</t>
+  </si>
+  <si>
+    <t>And Stock information</t>
+  </si>
+  <si>
+    <t>The MediaMarkt page should open</t>
+  </si>
+  <si>
+    <t>User must be able to click on personal care products</t>
+  </si>
+  <si>
+    <t>User should be able to click on male grooming products</t>
+  </si>
+  <si>
+    <t>The user should be able to rank the products from the most expensive to the least expensive.</t>
+  </si>
+  <si>
+    <t>User should be able to choose the most expensive product</t>
+  </si>
+  <si>
+    <t>The product must have an item number</t>
+  </si>
+  <si>
+    <t>The user should be able to click on the stock inquiry button</t>
+  </si>
+  <si>
+    <t>The user should be able to make stock inquiries</t>
+  </si>
+  <si>
+    <t>User should be able to see stock information</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -248,25 +333,7 @@
       <charset val="162"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="162"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="162"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="162"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Bahnschrift"/>
@@ -288,7 +355,7 @@
       <charset val="162"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
@@ -310,7 +377,7 @@
       <charset val="162"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Bahnschrift"/>
@@ -333,7 +400,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -341,85 +408,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="2">
+    <cellStyle name="Köprü" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -478,13 +496,29 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF202124"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
@@ -494,17 +528,17 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1628280</xdr:colOff>
+      <xdr:colOff>1247281</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>171000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="5 Resim" descr="mmarkt.PNG"/>
+        <xdr:cNvPr id="2" name="5 Resim" descr="mmarkt.PNG"/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -525,23 +559,23 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1189800</xdr:colOff>
+      <xdr:colOff>817266</xdr:colOff>
       <xdr:row>65</xdr:row>
       <xdr:rowOff>67680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1981080</xdr:colOff>
+      <xdr:colOff>1608547</xdr:colOff>
       <xdr:row>74</xdr:row>
       <xdr:rowOff>40320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="Resim 1" descr=""/>
+        <xdr:cNvPr id="3" name="Resim 1"/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -562,23 +596,23 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>2520000</xdr:colOff>
+      <xdr:colOff>2147467</xdr:colOff>
       <xdr:row>65</xdr:row>
       <xdr:rowOff>66240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>5696640</xdr:colOff>
+      <xdr:colOff>5324107</xdr:colOff>
       <xdr:row>74</xdr:row>
       <xdr:rowOff>44640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Resim 2" descr=""/>
+        <xdr:cNvPr id="4" name="Resim 2"/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -599,31 +633,289 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I156"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A59" activeCellId="0" sqref="A59"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H143" sqref="H143"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="65.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="33.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="83.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.57"/>
+    <col min="1" max="1" width="22.77734375" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" customWidth="1"/>
+    <col min="4" max="4" width="34.109375" customWidth="1"/>
+    <col min="5" max="5" width="65.6640625" customWidth="1"/>
+    <col min="6" max="6" width="33.44140625" customWidth="1"/>
+    <col min="7" max="7" width="89" customWidth="1"/>
+    <col min="8" max="8" width="26.109375" customWidth="1"/>
+    <col min="9" max="9" width="22.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -652,7 +944,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -681,7 +973,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E3" s="6" t="s">
         <v>17</v>
       </c>
@@ -693,7 +985,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E4" s="7" t="s">
         <v>19</v>
       </c>
@@ -705,7 +997,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E5" s="7" t="s">
         <v>21</v>
       </c>
@@ -716,7 +1008,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E6" s="6" t="s">
         <v>23</v>
       </c>
@@ -727,7 +1019,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E7" s="6" t="s">
         <v>25</v>
       </c>
@@ -738,7 +1030,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E8" s="6" t="s">
         <v>27</v>
       </c>
@@ -749,7 +1041,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E9" s="6" t="s">
         <v>29</v>
       </c>
@@ -760,7 +1052,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E10" s="6" t="s">
         <v>31</v>
       </c>
@@ -771,7 +1063,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E11" s="6" t="s">
         <v>33</v>
       </c>
@@ -782,7 +1074,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E12" s="6" t="s">
         <v>35</v>
       </c>
@@ -793,7 +1085,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E13" s="6" t="s">
         <v>37</v>
       </c>
@@ -804,82 +1096,82 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E15" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E16" s="9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E17" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E18" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E19" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E20" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E21" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E22" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E23" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E24" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E25" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E26" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E27" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E28" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="30" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -890,7 +1182,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>51</v>
       </c>
@@ -910,113 +1202,113 @@
       <c r="H31" s="6"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="H32" s="6"/>
       <c r="I32" s="3"/>
     </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="5:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
       <c r="H33" s="6"/>
       <c r="I33" s="3"/>
     </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="5:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E34" s="6"/>
       <c r="H34" s="8"/>
       <c r="I34" s="3"/>
     </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="5:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E35" s="6"/>
       <c r="H35" s="6"/>
       <c r="I35" s="3"/>
     </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="5:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E36" s="6"/>
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
       <c r="I36" s="3"/>
     </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="5:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E37" s="6"/>
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
       <c r="I37" s="3"/>
     </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="5:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E38" s="6"/>
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
       <c r="I38" s="3"/>
     </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="5:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E39" s="6"/>
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
       <c r="I39" s="3"/>
     </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="5:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E40" s="6"/>
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
       <c r="I40" s="3"/>
     </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="5:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E41" s="6"/>
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
       <c r="I41" s="3"/>
     </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="5:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E42" s="6"/>
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
       <c r="I42" s="3"/>
     </row>
-    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="5:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E44" s="9"/>
     </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="5:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E45" s="9"/>
     </row>
-    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="5:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E46" s="6"/>
     </row>
-    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="5:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E47" s="6"/>
     </row>
-    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="5:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E48" s="7"/>
     </row>
-    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E49" s="6"/>
     </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E50" s="6"/>
     </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E51" s="6"/>
     </row>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E52" s="6"/>
     </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E53" s="6"/>
     </row>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E54" s="6"/>
     </row>
-    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E55" s="6"/>
     </row>
-    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E56" s="6"/>
     </row>
-    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E57" s="6"/>
     </row>
-    <row r="58" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>0</v>
       </c>
@@ -1045,7 +1337,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:9" ht="60.6" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
         <v>53</v>
       </c>
@@ -1074,7 +1366,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E60" s="6" t="s">
         <v>17</v>
       </c>
@@ -1085,7 +1377,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:9" ht="30.6" x14ac:dyDescent="0.3">
       <c r="E61" s="7" t="s">
         <v>57</v>
       </c>
@@ -1096,7 +1388,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E62" s="6" t="s">
         <v>59</v>
       </c>
@@ -1107,7 +1399,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E63" s="6" t="s">
         <v>61</v>
       </c>
@@ -1118,7 +1410,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E64" s="6" t="s">
         <v>63</v>
       </c>
@@ -1129,38 +1421,38 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" spans="5:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E65" s="6"/>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="5:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E66" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" spans="5:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E67" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" spans="5:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E68" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" spans="5:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E69" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" spans="5:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E70" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" spans="5:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E71" s="6"/>
     </row>
-    <row r="85" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -1171,7 +1463,7 @@
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
     </row>
-    <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A86" s="6" t="s">
         <v>67</v>
       </c>
@@ -1188,7 +1480,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="120" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -1199,24 +1491,195 @@
       <c r="H120" s="1"/>
       <c r="I120" s="1"/>
     </row>
-    <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" spans="1:9" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A121" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B121" s="6" t="s">
         <v>54</v>
       </c>
       <c r="C121" s="7" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="D121" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="E121" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="F121" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="155" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G121" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H121" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I121" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E122" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G122" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H122" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E123" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G123" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H123" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E124" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G124" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H124" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E125" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G125" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H125" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E126" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G126" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H126" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E127" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G127" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="H127" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E128" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G128" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H128" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="129" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E129" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G129" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H129" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="130" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E130" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G130" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H130" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="132" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E132" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="133" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E133" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="134" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E134" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="135" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E135" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="136" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E136" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="137" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E137" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="138" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E138" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="139" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E139" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="140" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E140" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="141" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E141" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="142" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E142" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="143" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E143" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -1227,7 +1690,7 @@
       <c r="H155" s="1"/>
       <c r="I155" s="1"/>
     </row>
-    <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A156" s="6" t="s">
         <v>68</v>
       </c>
@@ -1246,26 +1709,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="https://www.mediamarkt.com.tr/"/>
-    <hyperlink ref="F2" r:id="rId2" display="https://www.mediamarkt.com.tr/"/>
-    <hyperlink ref="D31" r:id="rId3" display="https://www.mediamarkt.com.tr/"/>
-    <hyperlink ref="F31" r:id="rId4" display="https://www.mediamarkt.com.tr/"/>
-    <hyperlink ref="D59" r:id="rId5" display="https://www.mediamarkt.com.tr/"/>
-    <hyperlink ref="F59" r:id="rId6" display="https://www.mediamarkt.com.tr/"/>
-    <hyperlink ref="D86" r:id="rId7" display="https://www.mediamarkt.com.tr/"/>
-    <hyperlink ref="F86" r:id="rId8" display="https://www.mediamarkt.com.tr/"/>
-    <hyperlink ref="D121" r:id="rId9" display="https://www.mediamarkt.com.tr/"/>
-    <hyperlink ref="F121" r:id="rId10" display="https://www.mediamarkt.com.tr/"/>
-    <hyperlink ref="D156" r:id="rId11" display="https://www.mediamarkt.com.tr/"/>
-    <hyperlink ref="F156" r:id="rId12" display="https://www.mediamarkt.com.tr/"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId2"/>
+    <hyperlink ref="D31" r:id="rId3"/>
+    <hyperlink ref="F31" r:id="rId4"/>
+    <hyperlink ref="D59" r:id="rId5"/>
+    <hyperlink ref="F59" r:id="rId6"/>
+    <hyperlink ref="D86" r:id="rId7"/>
+    <hyperlink ref="F86" r:id="rId8"/>
+    <hyperlink ref="D121" r:id="rId9"/>
+    <hyperlink ref="F121" r:id="rId10"/>
+    <hyperlink ref="D156" r:id="rId11"/>
+    <hyperlink ref="F156" r:id="rId12"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <drawing r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId13"/>
+  <drawing r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>